<commit_message>
- Modificar el boton de eliminar test - Modificar el que aparezca o desaparezca el resultado final - Templates modificados de Virus detectados en español - Templates modificados de FLUID
</commit_message>
<xml_diff>
--- a/Template/Export/IndicDesemp_I1_11.xlsx
+++ b/Template/Export/IndicDesemp_I1_11.xlsx
@@ -39,9 +39,6 @@
     <t>Percentage of patients with reported virologic outcome</t>
   </si>
   <si>
-    <t>Percentage of SARI closed cases measured by the patient's egress condition variable</t>
-  </si>
-  <si>
     <t>Median days between clinical sample collection (DOC) and receipt (DOR) in the laboratory</t>
   </si>
   <si>
@@ -74,11 +71,14 @@
   <si>
     <t>Results</t>
   </si>
+  <si>
+    <t>Percentage of SARI closed cases</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -421,6 +421,12 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -440,12 +446,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -472,7 +472,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -520,6 +520,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-BBB9-4924-9EAE-4EDF66E721EC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -535,6 +540,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-BBB9-4924-9EAE-4EDF66E721EC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -551,6 +561,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-BBB9-4924-9EAE-4EDF66E721EC}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -569,6 +584,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-BBB9-4924-9EAE-4EDF66E721EC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -582,6 +602,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-BBB9-4924-9EAE-4EDF66E721EC}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -634,7 +659,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -646,7 +671,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -694,6 +719,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-3E72-4940-B792-EB4A76085DB8}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -709,6 +739,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-3E72-4940-B792-EB4A76085DB8}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -725,6 +760,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-3E72-4940-B792-EB4A76085DB8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -743,6 +783,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-3E72-4940-B792-EB4A76085DB8}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -756,6 +801,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-3E72-4940-B792-EB4A76085DB8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -797,7 +847,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -809,7 +859,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -857,6 +907,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-DF0C-45B3-B33F-0D2F177D22AE}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -872,6 +927,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-DF0C-45B3-B33F-0D2F177D22AE}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -888,6 +948,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-DF0C-45B3-B33F-0D2F177D22AE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -906,6 +971,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-DF0C-45B3-B33F-0D2F177D22AE}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -919,6 +989,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-DF0C-45B3-B33F-0D2F177D22AE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -960,7 +1035,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -972,7 +1047,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1020,6 +1095,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-97B6-4B70-A788-8011E1835B00}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1035,6 +1115,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-97B6-4B70-A788-8011E1835B00}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -1051,6 +1136,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-97B6-4B70-A788-8011E1835B00}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1069,6 +1159,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-97B6-4B70-A788-8011E1835B00}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -1082,6 +1177,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-97B6-4B70-A788-8011E1835B00}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1123,7 +1223,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1135,7 +1235,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1183,6 +1283,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-8E82-4059-966D-FD93FADFCA58}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1198,6 +1303,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-8E82-4059-966D-FD93FADFCA58}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -1214,6 +1324,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-8E82-4059-966D-FD93FADFCA58}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1232,6 +1347,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-8E82-4059-966D-FD93FADFCA58}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -1245,6 +1365,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-8E82-4059-966D-FD93FADFCA58}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1286,7 +1411,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1298,7 +1423,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1349,6 +1474,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-6F5C-4340-95BD-C9228A4B93B8}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1364,6 +1494,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-6F5C-4340-95BD-C9228A4B93B8}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -1380,6 +1515,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-6F5C-4340-95BD-C9228A4B93B8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1398,6 +1538,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-6F5C-4340-95BD-C9228A4B93B8}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -1411,6 +1556,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-6F5C-4340-95BD-C9228A4B93B8}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1452,7 +1602,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1464,7 +1614,7 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1507,6 +1657,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-06F9-4159-8E6D-64FF225113D3}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1522,6 +1677,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-06F9-4159-8E6D-64FF225113D3}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -1538,6 +1698,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-06F9-4159-8E6D-64FF225113D3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1577,6 +1742,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-06F9-4159-8E6D-64FF225113D3}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -1590,6 +1760,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-06F9-4159-8E6D-64FF225113D3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1631,7 +1806,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1643,7 +1818,7 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1686,6 +1861,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-79D4-4203-AA36-35569DF07C5D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1701,6 +1881,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-79D4-4203-AA36-35569DF07C5D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -1717,6 +1902,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-79D4-4203-AA36-35569DF07C5D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1756,6 +1946,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-79D4-4203-AA36-35569DF07C5D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -1769,6 +1964,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-79D4-4203-AA36-35569DF07C5D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1810,7 +2010,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6718,9 +6918,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:C6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6736,20 +6934,20 @@
   <sheetData>
     <row r="1" spans="2:9" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
-        <v>10</v>
+      <c r="B2" s="22" t="s">
+        <v>9</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="2:9" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -6761,7 +6959,7 @@
     </row>
     <row r="4" spans="2:9" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -6773,103 +6971,103 @@
     </row>
     <row r="5" spans="2:9" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:9" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="15" t="s">
+      <c r="E6" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="19"/>
+      <c r="F6" s="21"/>
     </row>
     <row r="7" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="13"/>
     </row>
     <row r="8" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
-        <v>4</v>
+      <c r="B9" s="18" t="s">
+        <v>15</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
-        <v>5</v>
+      <c r="B10" s="18" t="s">
+        <v>4</v>
       </c>
-      <c r="C10" s="17"/>
+      <c r="C10" s="19"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
-        <v>6</v>
+      <c r="B11" s="18" t="s">
+        <v>5</v>
       </c>
-      <c r="C11" s="17"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="6"/>
     </row>
     <row r="12" spans="2:9" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="23" t="s">
-        <v>7</v>
+      <c r="B12" s="16" t="s">
+        <v>6</v>
       </c>
-      <c r="C12" s="24"/>
+      <c r="C12" s="17"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="7"/>
     </row>
     <row r="13" spans="2:9" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="23" t="s">
-        <v>8</v>
+      <c r="B13" s="16" t="s">
+        <v>7</v>
       </c>
-      <c r="C13" s="24"/>
+      <c r="C13" s="17"/>
       <c r="D13" s="10"/>
       <c r="E13" s="14"/>
       <c r="F13" s="7"/>
     </row>
     <row r="14" spans="2:9" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="23" t="s">
-        <v>9</v>
+      <c r="B14" s="16" t="s">
+        <v>8</v>
       </c>
-      <c r="C14" s="24"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -6879,6 +7077,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">

</xml_diff>